<commit_message>
New 11-6-1-x files and titles
</commit_message>
<xml_diff>
--- a/hbar/11-4-1.xlsx
+++ b/hbar/11-4-1.xlsx
@@ -1,13 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <workbookPr defaultThemeVersion="202300"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleksey\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D490AE8D-99F8-4B35-AC31-A2171EB096A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="252" yWindow="1536" windowWidth="22788" windowHeight="10092" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Upstream tree" r:id="rId3" sheetId="1"/>
+    <sheet name="Upstream tree" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -371,20 +379,20 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -392,7 +400,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -409,1483 +417,1806 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="0E2841"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E8E8E8"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="156082"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="E97132"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="196B24"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="0F9ED5"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="A02B93"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="4EA72E"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="467886"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="96607D"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H161"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.9296875" customWidth="true"/>
-    <col min="2" max="2" width="2.9296875" customWidth="true"/>
-    <col min="3" max="3" width="2.9296875" customWidth="true"/>
-    <col min="4" max="4" width="2.9296875" customWidth="true"/>
-    <col min="5" max="5" width="2.9296875" customWidth="true"/>
-    <col min="6" max="6" width="49.8046875" customWidth="true"/>
-    <col min="7" max="7" width="24.90234375" customWidth="true"/>
-    <col min="8" max="8" width="24.90234375" customWidth="true"/>
+    <col min="1" max="5" width="2.88671875" customWidth="1"/>
+    <col min="6" max="6" width="49.77734375" customWidth="1"/>
+    <col min="7" max="8" width="24.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s" s="1">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G2" t="s" s="1">
+      <c r="G2" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="H2" t="s" s="1">
+      <c r="H2" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>-3176944.9434289746</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H3">
         <v>-2910235.4252200616</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>145349.29347330707</v>
       </c>
-      <c r="H4" t="n">
-        <v>98165.31252630918</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="H4">
+        <v>98165.312526309179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5">
         <v>22812.206403284363</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
         <v>5</v>
       </c>
-      <c r="G6" t="n">
-        <v>22662.25634361289</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="G6">
+        <v>22662.256343612891</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E7" t="s">
         <v>6</v>
       </c>
-      <c r="G7" t="n">
-        <v>5803.265940485628</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="G7">
+        <v>5803.2659404856277</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F8" t="s">
         <v>7</v>
       </c>
-      <c r="G8" t="n">
-        <v>5803.265940485629</v>
-      </c>
-      <c r="H8" t="n">
-        <v>4630.832431951792</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="G8">
+        <v>5803.2659404856286</v>
+      </c>
+      <c r="H8">
+        <v>4630.8324319517924</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E9" t="s">
         <v>8</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G9">
         <v>5213.4036207884565</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F10" t="s">
         <v>9</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G10">
         <v>2192.4588056041785</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F11" t="s">
         <v>10</v>
       </c>
-      <c r="G11" t="n">
+      <c r="G11">
         <v>1473.58109597661</v>
       </c>
-      <c r="H11" t="n">
+      <c r="H11">
         <v>7.4896647328351005</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F12" t="s">
         <v>11</v>
       </c>
-      <c r="G12" t="n">
-        <v>671.8331207431922</v>
-      </c>
-    </row>
-    <row r="13">
+      <c r="G12">
+        <v>671.83312074319224</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F13" t="s">
         <v>12</v>
       </c>
-      <c r="G13" t="n">
+      <c r="G13">
         <v>466.94966083256423</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E14" t="s">
         <v>13</v>
       </c>
-      <c r="G14" t="n">
+      <c r="G14">
         <v>3385.2818407801974</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F15" t="s">
         <v>14</v>
       </c>
-      <c r="G15" t="n">
-        <v>1957.626425652264</v>
-      </c>
-    </row>
-    <row r="16">
+      <c r="G15">
+        <v>1957.6264256522641</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F16" t="s">
         <v>15</v>
       </c>
-      <c r="G16" t="n">
-        <v>787.6950628779692</v>
-      </c>
-    </row>
-    <row r="17">
+      <c r="G16">
+        <v>787.69506287796924</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
       <c r="F17" t="s">
         <v>16</v>
       </c>
-      <c r="G17" t="n">
+      <c r="G17">
         <v>352.2585789092247</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
       <c r="E18" t="s">
         <v>17</v>
       </c>
-      <c r="G18" t="n">
+      <c r="G18">
         <v>3199.6814103854085</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
       <c r="F19" t="s">
         <v>18</v>
       </c>
-      <c r="G19" t="n">
+      <c r="G19">
         <v>2100.4618590989426</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.3">
       <c r="F20" t="s">
         <v>19</v>
       </c>
-      <c r="G20" t="n">
+      <c r="G20">
         <v>1032.2346208909312</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.3">
       <c r="E21" t="s">
         <v>20</v>
       </c>
-      <c r="G21" t="n">
+      <c r="G21">
         <v>1883.6570135407248</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.3">
       <c r="F22" t="s">
         <v>21</v>
       </c>
-      <c r="G22" t="n">
-        <v>971.6722808613526</v>
-      </c>
-    </row>
-    <row r="23">
+      <c r="G22">
+        <v>971.67228086135265</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.3">
       <c r="F23" t="s">
         <v>22</v>
       </c>
-      <c r="G23" t="n">
+      <c r="G23">
         <v>454.69666508658923</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.3">
       <c r="E24" t="s">
         <v>23</v>
       </c>
-      <c r="G24" t="n">
+      <c r="G24">
         <v>1600.6115118103273</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.3">
       <c r="F25" t="s">
         <v>24</v>
       </c>
-      <c r="G25" t="n">
+      <c r="G25">
         <v>1007.3331735338234</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.3">
       <c r="F26" t="s">
         <v>15</v>
       </c>
-      <c r="G26" t="n">
+      <c r="G26">
         <v>485.57032814200403</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.3">
       <c r="E27" t="s">
         <v>25</v>
       </c>
-      <c r="G27" t="n">
-        <v>1322.478925577438</v>
-      </c>
-    </row>
-    <row r="28">
+      <c r="G27">
+        <v>1322.4789255774381</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.3">
       <c r="F28" t="s">
         <v>26</v>
       </c>
-      <c r="G28" t="n">
-        <v>868.1133595929438</v>
-      </c>
-    </row>
-    <row r="29">
+      <c r="G28">
+        <v>868.11335959294377</v>
+      </c>
+    </row>
+    <row r="29" spans="3:7" x14ac:dyDescent="0.3">
       <c r="F29" t="s">
         <v>27</v>
       </c>
-      <c r="G29" t="n">
-        <v>428.7247654551559</v>
-      </c>
-    </row>
-    <row r="30">
+      <c r="G29">
+        <v>428.72476545515588</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
         <v>28</v>
       </c>
-      <c r="G30" t="n">
+      <c r="G30">
         <v>18129.455429691967</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D31" t="s">
         <v>29</v>
       </c>
-      <c r="G31" t="n">
-        <v>18020.31310988856</v>
-      </c>
-    </row>
-    <row r="32">
+      <c r="G31">
+        <v>18020.313109888561</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.3">
       <c r="E32" t="s">
         <v>30</v>
       </c>
-      <c r="G32" t="n">
+      <c r="G32">
         <v>17081.90486813302</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F33" t="s">
         <v>31</v>
       </c>
-      <c r="G33" t="n">
+      <c r="G33">
         <v>16661.54602682123</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E34" t="s">
         <v>32</v>
       </c>
-      <c r="G34" t="n">
+      <c r="G34">
         <v>323.51982059180057</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
         <v>33</v>
       </c>
-      <c r="G35" t="n">
+      <c r="G35">
         <v>3673.7727233269475</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D36" t="s">
         <v>34</v>
       </c>
-      <c r="G36" t="n">
+      <c r="G36">
         <v>2511.1596360566987</v>
       </c>
-      <c r="H36" t="n">
-        <v>66.01388174760359</v>
-      </c>
-    </row>
-    <row r="37">
+      <c r="H36">
+        <v>66.013881747603591</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E37" t="s">
         <v>25</v>
       </c>
-      <c r="G37" t="n">
-        <v>519.2794900709503</v>
-      </c>
-    </row>
-    <row r="38">
+      <c r="G37">
+        <v>519.27949007095026</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F38" t="s">
         <v>26</v>
       </c>
-      <c r="G38" t="n">
+      <c r="G38">
         <v>340.87005393781374</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E39" t="s">
         <v>8</v>
       </c>
-      <c r="G39" t="n">
+      <c r="G39">
         <v>373.90821614068665</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D40" t="s">
         <v>35</v>
       </c>
-      <c r="G40" t="n">
+      <c r="G40">
         <v>1162.6130872702502</v>
       </c>
-      <c r="H40" t="n">
-        <v>32.60148649514664</v>
-      </c>
-    </row>
-    <row r="41">
+      <c r="H40">
+        <v>32.601486495146638</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
         <v>36</v>
       </c>
-      <c r="G41" t="n">
+      <c r="G41">
         <v>2568.5463906945624</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D42" t="s">
         <v>37</v>
       </c>
-      <c r="G42" t="n">
-        <v>2559.892162841726</v>
-      </c>
-    </row>
-    <row r="43">
+      <c r="G42">
+        <v>2559.8921628417261</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E43" t="s">
         <v>38</v>
       </c>
-      <c r="G43" t="n">
+      <c r="G43">
         <v>1072.5339076459043</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F44" t="s">
         <v>39</v>
       </c>
-      <c r="G44" t="n">
+      <c r="G44">
         <v>1057.2483965798954</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E45" t="s">
         <v>40</v>
       </c>
-      <c r="G45" t="n">
-        <v>555.4611395144958</v>
-      </c>
-    </row>
-    <row r="46">
+      <c r="G45">
+        <v>555.46113951449581</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E46" t="s">
         <v>41</v>
       </c>
-      <c r="G46" t="n">
-        <v>504.3301398032933</v>
-      </c>
-    </row>
-    <row r="47">
+      <c r="G46">
+        <v>504.33013980329332</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F47" t="s">
         <v>42</v>
       </c>
-      <c r="G47" t="n">
+      <c r="G47">
         <v>336.80496111274454</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>43</v>
       </c>
-      <c r="G48" t="n">
+      <c r="G48">
         <v>27062.767959999997</v>
       </c>
-      <c r="H48" t="n">
-        <v>27062.76796</v>
-      </c>
-    </row>
-    <row r="49">
+      <c r="H48">
+        <v>27062.767960000001</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>44</v>
       </c>
-      <c r="G49" t="n">
+      <c r="G49">
         <v>-1685.959809655182</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C50" t="s">
         <v>15</v>
       </c>
-      <c r="G50" t="n">
-        <v>-778.2907075372015</v>
-      </c>
-    </row>
-    <row r="51">
+      <c r="G50">
+        <v>-778.29070753720146</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C51" t="s">
         <v>45</v>
       </c>
-      <c r="G51" t="n">
-        <v>-900.0293551593957</v>
-      </c>
-    </row>
-    <row r="52">
+      <c r="G51">
+        <v>-900.02935515939566</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D52" t="s">
         <v>6</v>
       </c>
-      <c r="G52" t="n">
-        <v>-838.281589711208</v>
-      </c>
-    </row>
-    <row r="53">
+      <c r="G52">
+        <v>-838.28158971120797</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E53" t="s">
         <v>7</v>
       </c>
-      <c r="G53" t="n">
-        <v>-838.2815897112081</v>
-      </c>
-      <c r="H53" t="n">
-        <v>-668.9236048379199</v>
-      </c>
-    </row>
-    <row r="54">
+      <c r="G53">
+        <v>-838.28158971120808</v>
+      </c>
+      <c r="H53">
+        <v>-668.92360483791992</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>46</v>
       </c>
-      <c r="G54" t="n">
+      <c r="G54">
         <v>-16989.678189105085</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C55" t="s">
         <v>15</v>
       </c>
-      <c r="G55" t="n">
+      <c r="G55">
         <v>-1118.9935613792888</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D56" t="s">
         <v>47</v>
       </c>
-      <c r="G56" t="n">
+      <c r="G56">
         <v>-367.0530351977435</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C57" t="s">
         <v>48</v>
       </c>
-      <c r="G57" t="n">
+      <c r="G57">
         <v>-15844.177256337527</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D58" t="s">
         <v>49</v>
       </c>
-      <c r="G58" t="n">
-        <v>-848.485214422155</v>
-      </c>
-      <c r="H58" t="n">
-        <v>-731.5091836433778</v>
-      </c>
-    </row>
-    <row r="59">
+      <c r="G58">
+        <v>-848.48521442215497</v>
+      </c>
+      <c r="H58">
+        <v>-731.50918364337781</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D59" t="s">
         <v>50</v>
       </c>
-      <c r="G59" t="n">
+      <c r="G59">
         <v>-1236.5421120735064</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E60" t="s">
         <v>51</v>
       </c>
-      <c r="G60" t="n">
+      <c r="G60">
         <v>-1228.1004746083515</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F61" t="s">
         <v>52</v>
       </c>
-      <c r="G61" t="n">
+      <c r="G61">
         <v>-916.9978971940244</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D62" t="s">
         <v>53</v>
       </c>
-      <c r="G62" t="n">
-        <v>-3265.693678458541</v>
-      </c>
-      <c r="H62" t="n">
+      <c r="G62">
+        <v>-3265.6936784585409</v>
+      </c>
+      <c r="H62">
         <v>-2720.8760017905392</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E63" t="s">
         <v>54</v>
       </c>
-      <c r="G63" t="n">
-        <v>-377.1120385676741</v>
-      </c>
-    </row>
-    <row r="64">
+      <c r="G63">
+        <v>-377.11203856767412</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D64" t="s">
         <v>38</v>
       </c>
-      <c r="G64" t="n">
-        <v>-4905.433438515865</v>
-      </c>
-    </row>
-    <row r="65">
+      <c r="G64">
+        <v>-4905.4334385158654</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E65" t="s">
         <v>39</v>
       </c>
-      <c r="G65" t="n">
-        <v>-4835.522308831786</v>
-      </c>
-    </row>
-    <row r="66">
+      <c r="G65">
+        <v>-4835.5223088317862</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F66" t="s">
         <v>49</v>
       </c>
-      <c r="G66" t="n">
+      <c r="G66">
         <v>-318.29277789375084</v>
       </c>
-      <c r="H66" t="n">
+      <c r="H66">
         <v>-274.41148785981846</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F67" t="s">
         <v>55</v>
       </c>
-      <c r="G67" t="n">
-        <v>-4311.61905894624</v>
-      </c>
-      <c r="H67" t="n">
+      <c r="G67">
+        <v>-4311.6190589462403</v>
+      </c>
+      <c r="H67">
         <v>-3356.8628115924325</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D68" t="s">
         <v>8</v>
       </c>
-      <c r="G68" t="n">
-        <v>-5129.107310265196</v>
-      </c>
-    </row>
-    <row r="69">
+      <c r="G68">
+        <v>-5129.1073102651962</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E69" t="s">
         <v>12</v>
       </c>
-      <c r="G69" t="n">
+      <c r="G69">
         <v>-459.3994812433001</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F70" t="s">
         <v>56</v>
       </c>
-      <c r="G70" t="n">
+      <c r="G70">
         <v>-457.23572489752536</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E71" t="s">
         <v>11</v>
       </c>
-      <c r="G71" t="n">
-        <v>-660.9701495471479</v>
-      </c>
-    </row>
-    <row r="72">
+      <c r="G71">
+        <v>-660.97014954714791</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F72" t="s">
         <v>57</v>
       </c>
-      <c r="G72" t="n">
+      <c r="G72">
         <v>-625.4631361792359</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E73" t="s">
         <v>10</v>
       </c>
-      <c r="G73" t="n">
+      <c r="G73">
         <v>-1449.7545406812683</v>
       </c>
-      <c r="H73" t="n">
-        <v>-7.368563212608149</v>
-      </c>
-    </row>
-    <row r="74">
+      <c r="H73">
+        <v>-7.3685632126081488</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F74" t="s">
         <v>58</v>
       </c>
-      <c r="G74" t="n">
+      <c r="G74">
         <v>-1439.7264443886997</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E75" t="s">
         <v>9</v>
       </c>
-      <c r="G75" t="n">
-        <v>-2157.008608049991</v>
-      </c>
-    </row>
-    <row r="76">
+      <c r="G75">
+        <v>-2157.0086080499909</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F76" t="s">
         <v>59</v>
       </c>
-      <c r="G76" t="n">
+      <c r="G76">
         <v>-334.7458147600712</v>
       </c>
-      <c r="H76" t="n">
+      <c r="H76">
         <v>-1.8176579189576014</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F77" t="s">
         <v>60</v>
       </c>
-      <c r="G77" t="n">
+      <c r="G77">
         <v>-1316.8393908137714</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
         <v>61</v>
       </c>
-      <c r="G78" t="n">
-        <v>-420445.9416434611</v>
-      </c>
-    </row>
-    <row r="79">
+      <c r="G78">
+        <v>-420445.94164346112</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C79" t="s">
         <v>62</v>
       </c>
-      <c r="G79" t="n">
-        <v>-9369.04462255181</v>
-      </c>
-      <c r="H79" t="n">
+      <c r="G79">
+        <v>-9369.0446225518099</v>
+      </c>
+      <c r="H79">
         <v>-25.016127284098115</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D80" t="s">
         <v>63</v>
       </c>
-      <c r="G80" t="n">
-        <v>-9338.83324907296</v>
-      </c>
-    </row>
-    <row r="81">
+      <c r="G80">
+        <v>-9338.8332490729608</v>
+      </c>
+    </row>
+    <row r="81" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E81" t="s">
         <v>64</v>
       </c>
-      <c r="G81" t="n">
-        <v>-9277.705785217673</v>
-      </c>
-      <c r="H81" t="n">
+      <c r="G81">
+        <v>-9277.7057852176731</v>
+      </c>
+      <c r="H81">
         <v>-12.85693820737151</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="3:8" x14ac:dyDescent="0.3">
       <c r="F82" t="s">
         <v>65</v>
       </c>
-      <c r="G82" t="n">
+      <c r="G82">
         <v>-372.39639743951255</v>
       </c>
-      <c r="H82" t="n">
-        <v>-372.3209697021316</v>
-      </c>
-    </row>
-    <row r="83">
+      <c r="H82">
+        <v>-372.32096970213161</v>
+      </c>
+    </row>
+    <row r="83" spans="3:8" x14ac:dyDescent="0.3">
       <c r="F83" t="s">
         <v>66</v>
       </c>
-      <c r="G83" t="n">
+      <c r="G83">
         <v>-3447.9702975502987</v>
       </c>
-      <c r="H83" t="n">
-        <v>-3348.070244829342</v>
-      </c>
-    </row>
-    <row r="84">
+      <c r="H83">
+        <v>-3348.0702448293418</v>
+      </c>
+    </row>
+    <row r="84" spans="3:8" x14ac:dyDescent="0.3">
       <c r="F84" t="s">
         <v>67</v>
       </c>
-      <c r="G84" t="n">
+      <c r="G84">
         <v>-4707.6808008022745</v>
       </c>
-      <c r="H84" t="n">
-        <v>-4047.408668959764</v>
-      </c>
-    </row>
-    <row r="85">
+      <c r="H84">
+        <v>-4047.4086689597639</v>
+      </c>
+    </row>
+    <row r="85" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C85" t="s">
         <v>68</v>
       </c>
-      <c r="G85" t="n">
+      <c r="G85">
         <v>-32701.471973845088</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="3:8" x14ac:dyDescent="0.3">
       <c r="D86" t="s">
         <v>69</v>
       </c>
-      <c r="G86" t="n">
+      <c r="G86">
         <v>-451.93139368327985</v>
       </c>
-      <c r="H86" t="n">
+      <c r="H86">
         <v>-108.7782837422518</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="3:8" x14ac:dyDescent="0.3">
       <c r="D87" t="s">
         <v>70</v>
       </c>
-      <c r="G87" t="n">
-        <v>-873.7540868664038</v>
-      </c>
-      <c r="H87" t="n">
-        <v>-86.83093168436874</v>
-      </c>
-    </row>
-    <row r="88">
+      <c r="G87">
+        <v>-873.75408686640378</v>
+      </c>
+      <c r="H87">
+        <v>-86.830931684368736</v>
+      </c>
+    </row>
+    <row r="88" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E88" t="s">
         <v>71</v>
       </c>
-      <c r="G88" t="n">
+      <c r="G88">
         <v>-431.03363261437937</v>
       </c>
-      <c r="H88" t="n">
+      <c r="H88">
         <v>-1.6382290063700802</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="3:8" x14ac:dyDescent="0.3">
       <c r="D89" t="s">
         <v>72</v>
       </c>
-      <c r="G89" t="n">
+      <c r="G89">
         <v>-1005.9816150125054</v>
       </c>
-      <c r="H89" t="n">
-        <v>-77.89510068832924</v>
-      </c>
-    </row>
-    <row r="90">
+      <c r="H89">
+        <v>-77.895100688329237</v>
+      </c>
+    </row>
+    <row r="90" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E90" t="s">
         <v>73</v>
       </c>
-      <c r="G90" t="n">
-        <v>-564.9753109245127</v>
-      </c>
-      <c r="H90" t="n">
-        <v>-1.500426359823508</v>
-      </c>
-    </row>
-    <row r="91">
+      <c r="G90">
+        <v>-564.97531092451266</v>
+      </c>
+      <c r="H90">
+        <v>-1.5004263598235079</v>
+      </c>
+    </row>
+    <row r="91" spans="3:8" x14ac:dyDescent="0.3">
       <c r="D91" t="s">
         <v>74</v>
       </c>
-      <c r="G91" t="n">
+      <c r="G91">
         <v>-1384.3015008285633</v>
       </c>
-      <c r="H91" t="n">
+      <c r="H91">
         <v>-107.17326090712058</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E92" t="s">
         <v>75</v>
       </c>
-      <c r="G92" t="n">
+      <c r="G92">
         <v>-405.04153290716437</v>
       </c>
-      <c r="H92" t="n">
-        <v>-5.327876722002068</v>
-      </c>
-    </row>
-    <row r="93">
+      <c r="H92">
+        <v>-5.3278767220020677</v>
+      </c>
+    </row>
+    <row r="93" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E93" t="s">
         <v>76</v>
       </c>
-      <c r="G93" t="n">
-        <v>-536.425836215542</v>
-      </c>
-    </row>
-    <row r="94">
+      <c r="G93">
+        <v>-536.42583621554195</v>
+      </c>
+    </row>
+    <row r="94" spans="3:8" x14ac:dyDescent="0.3">
       <c r="F94" t="s">
         <v>77</v>
       </c>
-      <c r="G94" t="n">
-        <v>-536.4258362155417</v>
-      </c>
-    </row>
-    <row r="95">
+      <c r="G94">
+        <v>-536.42583621554172</v>
+      </c>
+    </row>
+    <row r="95" spans="3:8" x14ac:dyDescent="0.3">
       <c r="D95" t="s">
         <v>78</v>
       </c>
-      <c r="G95" t="n">
-        <v>-6387.27896201641</v>
-      </c>
-      <c r="H95" t="n">
-        <v>-672.7475140607131</v>
-      </c>
-    </row>
-    <row r="96">
+      <c r="G95">
+        <v>-6387.2789620164103</v>
+      </c>
+      <c r="H95">
+        <v>-672.74751406071312</v>
+      </c>
+    </row>
+    <row r="96" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E96" t="s">
         <v>79</v>
       </c>
-      <c r="G96" t="n">
+      <c r="G96">
         <v>-346.28801765389454</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E97" t="s">
         <v>76</v>
       </c>
-      <c r="G97" t="n">
-        <v>-1091.30419956496</v>
-      </c>
-    </row>
-    <row r="98">
+      <c r="G97">
+        <v>-1091.3041995649601</v>
+      </c>
+    </row>
+    <row r="98" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F98" t="s">
         <v>77</v>
       </c>
-      <c r="G98" t="n">
+      <c r="G98">
         <v>-1091.3041995649596</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E99" t="s">
         <v>80</v>
       </c>
-      <c r="G99" t="n">
+      <c r="G99">
         <v>-3840.2834376613687</v>
       </c>
-      <c r="H99" t="n">
-        <v>-8.022911911212535</v>
-      </c>
-    </row>
-    <row r="100">
+      <c r="H99">
+        <v>-8.0229119112125353</v>
+      </c>
+    </row>
+    <row r="100" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F100" t="s">
         <v>81</v>
       </c>
-      <c r="G100" t="n">
+      <c r="G100">
         <v>-1025.2833535241048</v>
       </c>
-      <c r="H100" t="n">
-        <v>-861.4589613440074</v>
-      </c>
-    </row>
-    <row r="101">
+      <c r="H100">
+        <v>-861.45896134400743</v>
+      </c>
+    </row>
+    <row r="101" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F101" t="s">
         <v>82</v>
       </c>
-      <c r="G101" t="n">
+      <c r="G101">
         <v>-1781.5533189966202</v>
       </c>
-      <c r="H101" t="n">
-        <v>-1725.67261128647</v>
-      </c>
-    </row>
-    <row r="102">
+      <c r="H101">
+        <v>-1725.6726112864701</v>
+      </c>
+    </row>
+    <row r="102" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D102" t="s">
         <v>83</v>
       </c>
-      <c r="G102" t="n">
-        <v>-11136.18150009918</v>
-      </c>
-      <c r="H102" t="n">
-        <v>-558.1933680158866</v>
-      </c>
-    </row>
-    <row r="103">
+      <c r="G102">
+        <v>-11136.181500099179</v>
+      </c>
+      <c r="H102">
+        <v>-558.19336801588656</v>
+      </c>
+    </row>
+    <row r="103" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E103" t="s">
         <v>84</v>
       </c>
-      <c r="G103" t="n">
-        <v>-696.3376110239168</v>
-      </c>
-    </row>
-    <row r="104">
+      <c r="G103">
+        <v>-696.33761102391679</v>
+      </c>
+    </row>
+    <row r="104" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F104" t="s">
         <v>85</v>
       </c>
-      <c r="G104" t="n">
-        <v>-524.6581308126162</v>
-      </c>
-    </row>
-    <row r="105">
+      <c r="G104">
+        <v>-524.65813081261615</v>
+      </c>
+    </row>
+    <row r="105" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E105" t="s">
         <v>79</v>
       </c>
-      <c r="G105" t="n">
-        <v>-875.8661862729475</v>
-      </c>
-    </row>
-    <row r="106">
+      <c r="G105">
+        <v>-875.86618627294752</v>
+      </c>
+    </row>
+    <row r="106" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F106" t="s">
         <v>86</v>
       </c>
-      <c r="G106" t="n">
-        <v>-599.4766807214231</v>
-      </c>
-    </row>
-    <row r="107">
+      <c r="G106">
+        <v>-599.47668072142312</v>
+      </c>
+    </row>
+    <row r="107" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E107" t="s">
         <v>76</v>
       </c>
-      <c r="G107" t="n">
+      <c r="G107">
         <v>-2976.0813036683035</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F108" t="s">
         <v>77</v>
       </c>
-      <c r="G108" t="n">
-        <v>-2976.081303668302</v>
-      </c>
-    </row>
-    <row r="109">
+      <c r="G108">
+        <v>-2976.0813036683021</v>
+      </c>
+    </row>
+    <row r="109" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E109" t="s">
         <v>87</v>
       </c>
-      <c r="G109" t="n">
-        <v>-5818.718646546027</v>
-      </c>
-    </row>
-    <row r="110">
+      <c r="G109">
+        <v>-5818.7186465460272</v>
+      </c>
+    </row>
+    <row r="110" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F110" t="s">
         <v>88</v>
       </c>
-      <c r="G110" t="n">
+      <c r="G110">
         <v>-394.13177143136573</v>
       </c>
-      <c r="H110" t="n">
-        <v>-1.239187409371891</v>
-      </c>
-    </row>
-    <row r="111">
+      <c r="H110">
+        <v>-1.2391874093718911</v>
+      </c>
+    </row>
+    <row r="111" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F111" t="s">
         <v>89</v>
       </c>
-      <c r="G111" t="n">
+      <c r="G111">
         <v>-436.8882447334218</v>
       </c>
-      <c r="H111" t="n">
-        <v>-0.8560622085178525</v>
-      </c>
-    </row>
-    <row r="112">
+      <c r="H111">
+        <v>-0.85606220851785253</v>
+      </c>
+    </row>
+    <row r="112" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F112" t="s">
         <v>64</v>
       </c>
-      <c r="G112" t="n">
+      <c r="G112">
         <v>-508.21609611337516</v>
       </c>
-      <c r="H112" t="n">
-        <v>-0.7042800337700018</v>
-      </c>
-    </row>
-    <row r="113">
+      <c r="H112">
+        <v>-0.70428003377000181</v>
+      </c>
+    </row>
+    <row r="113" spans="3:8" x14ac:dyDescent="0.3">
       <c r="F113" t="s">
         <v>73</v>
       </c>
-      <c r="G113" t="n">
-        <v>-513.5286117843312</v>
-      </c>
-      <c r="H113" t="n">
+      <c r="G113">
+        <v>-513.52861178433125</v>
+      </c>
+      <c r="H113">
         <v>-1.3637974098088208</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" spans="3:8" x14ac:dyDescent="0.3">
       <c r="F114" t="s">
         <v>90</v>
       </c>
-      <c r="G114" t="n">
-        <v>-706.2989708161209</v>
-      </c>
-      <c r="H114" t="n">
+      <c r="G114">
+        <v>-706.29897081612091</v>
+      </c>
+      <c r="H114">
         <v>-1.5929408314100268</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" spans="3:8" x14ac:dyDescent="0.3">
       <c r="F115" t="s">
         <v>80</v>
       </c>
-      <c r="G115" t="n">
+      <c r="G115">
         <v>-1239.9012501939144</v>
       </c>
-      <c r="H115" t="n">
-        <v>-2.590334455877014</v>
-      </c>
-    </row>
-    <row r="116">
+      <c r="H115">
+        <v>-2.5903344558770138</v>
+      </c>
+    </row>
+    <row r="116" spans="3:8" x14ac:dyDescent="0.3">
       <c r="D116" t="s">
         <v>91</v>
       </c>
-      <c r="G116" t="n">
+      <c r="G116">
         <v>-11462.042915338747</v>
       </c>
-      <c r="H116" t="n">
-        <v>-6682.892133139035</v>
-      </c>
-    </row>
-    <row r="117">
+      <c r="H116">
+        <v>-6682.8921331390347</v>
+      </c>
+    </row>
+    <row r="117" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E117" t="s">
         <v>84</v>
       </c>
-      <c r="G117" t="n">
-        <v>-540.6313506720109</v>
-      </c>
-    </row>
-    <row r="118">
+      <c r="G117">
+        <v>-540.63135067201085</v>
+      </c>
+    </row>
+    <row r="118" spans="3:8" x14ac:dyDescent="0.3">
       <c r="F118" t="s">
         <v>85</v>
       </c>
-      <c r="G118" t="n">
+      <c r="G118">
         <v>-407.34067701038623</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E119" t="s">
         <v>79</v>
       </c>
-      <c r="G119" t="n">
-        <v>-680.0160034389165</v>
-      </c>
-    </row>
-    <row r="120">
+      <c r="G119">
+        <v>-680.01600343891653</v>
+      </c>
+    </row>
+    <row r="120" spans="3:8" x14ac:dyDescent="0.3">
       <c r="F120" t="s">
         <v>86</v>
       </c>
-      <c r="G120" t="n">
-        <v>-465.4292436081917</v>
-      </c>
-    </row>
-    <row r="121">
+      <c r="G120">
+        <v>-465.42924360819171</v>
+      </c>
+    </row>
+    <row r="121" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E121" t="s">
         <v>31</v>
       </c>
-      <c r="G121" t="n">
-        <v>-1157.313721639378</v>
-      </c>
-    </row>
-    <row r="122">
+      <c r="G121">
+        <v>-1157.3137216393779</v>
+      </c>
+    </row>
+    <row r="122" spans="3:8" x14ac:dyDescent="0.3">
       <c r="F122" t="s">
         <v>92</v>
       </c>
-      <c r="G122" t="n">
+      <c r="G122">
         <v>-1092.1317311485222</v>
       </c>
-      <c r="H122" t="n">
-        <v>-3.251597636574705</v>
-      </c>
-    </row>
-    <row r="123">
+      <c r="H122">
+        <v>-3.2515976365747048</v>
+      </c>
+    </row>
+    <row r="123" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E123" t="s">
         <v>76</v>
       </c>
-      <c r="G123" t="n">
+      <c r="G123">
         <v>-2310.6074258232925</v>
       </c>
     </row>
-    <row r="124">
+    <row r="124" spans="3:8" x14ac:dyDescent="0.3">
       <c r="F124" t="s">
         <v>77</v>
       </c>
-      <c r="G124" t="n">
+      <c r="G124">
         <v>-2310.6074258232916</v>
       </c>
     </row>
-    <row r="125">
+    <row r="125" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C125" t="s">
         <v>93</v>
       </c>
-      <c r="G125" t="n">
+      <c r="G125">
         <v>-378375.42504706414</v>
       </c>
-      <c r="H125" t="n">
-        <v>-299177.4745731485</v>
-      </c>
-    </row>
-    <row r="126">
+      <c r="H125">
+        <v>-299177.47457314847</v>
+      </c>
+    </row>
+    <row r="126" spans="3:8" x14ac:dyDescent="0.3">
       <c r="D126" t="s">
         <v>94</v>
       </c>
-      <c r="G126" t="n">
-        <v>-537.3182730866698</v>
-      </c>
-    </row>
-    <row r="127">
+      <c r="G126">
+        <v>-537.31827308666982</v>
+      </c>
+    </row>
+    <row r="127" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E127" t="s">
         <v>95</v>
       </c>
-      <c r="G127" t="n">
+      <c r="G127">
         <v>-359.6849616081808</v>
       </c>
     </row>
-    <row r="128">
+    <row r="128" spans="3:8" x14ac:dyDescent="0.3">
       <c r="F128" t="s">
         <v>96</v>
       </c>
-      <c r="G128" t="n">
-        <v>-359.6849616081803</v>
-      </c>
-    </row>
-    <row r="129">
+      <c r="G128">
+        <v>-359.68496160818029</v>
+      </c>
+    </row>
+    <row r="129" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D129" t="s">
         <v>6</v>
       </c>
-      <c r="G129" t="n">
+      <c r="G129">
         <v>-2689.1073206009896</v>
       </c>
     </row>
-    <row r="130">
+    <row r="130" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E130" t="s">
         <v>7</v>
       </c>
-      <c r="G130" t="n">
-        <v>-2689.10732060099</v>
-      </c>
-      <c r="H130" t="n">
+      <c r="G130">
+        <v>-2689.1073206009901</v>
+      </c>
+      <c r="H130">
         <v>-2145.827111999623</v>
       </c>
     </row>
-    <row r="131">
+    <row r="131" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F131" t="s">
         <v>97</v>
       </c>
-      <c r="G131" t="n">
-        <v>-381.6727709481083</v>
-      </c>
-    </row>
-    <row r="132">
+      <c r="G131">
+        <v>-381.67277094810828</v>
+      </c>
+    </row>
+    <row r="132" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D132" t="s">
         <v>98</v>
       </c>
-      <c r="G132" t="n">
-        <v>-6060.547260747401</v>
-      </c>
-    </row>
-    <row r="133">
+      <c r="G132">
+        <v>-6060.5472607474012</v>
+      </c>
+    </row>
+    <row r="133" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E133" t="s">
         <v>99</v>
       </c>
-      <c r="G133" t="n">
-        <v>-519.9803431147596</v>
-      </c>
-    </row>
-    <row r="134">
+      <c r="G133">
+        <v>-519.98034311475965</v>
+      </c>
+    </row>
+    <row r="134" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E134" t="s">
         <v>100</v>
       </c>
-      <c r="G134" t="n">
+      <c r="G134">
         <v>-5540.5669176326355</v>
       </c>
     </row>
-    <row r="135">
+    <row r="135" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F135" t="s">
         <v>8</v>
       </c>
-      <c r="G135" t="n">
+      <c r="G135">
         <v>-368.14195326321965</v>
       </c>
     </row>
-    <row r="136">
+    <row r="136" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F136" t="s">
         <v>101</v>
       </c>
-      <c r="G136" t="n">
-        <v>-602.4870631560382</v>
-      </c>
-    </row>
-    <row r="137">
+      <c r="G136">
+        <v>-602.48706315603818</v>
+      </c>
+    </row>
+    <row r="137" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F137" t="s">
         <v>94</v>
       </c>
-      <c r="G137" t="n">
+      <c r="G137">
         <v>-653.5994248023826</v>
       </c>
     </row>
-    <row r="138">
+    <row r="138" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F138" t="s">
         <v>6</v>
       </c>
-      <c r="G138" t="n">
-        <v>-668.879931045566</v>
-      </c>
-    </row>
-    <row r="139">
+      <c r="G138">
+        <v>-668.87993104556597</v>
+      </c>
+    </row>
+    <row r="139" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F139" t="s">
         <v>102</v>
       </c>
-      <c r="G139" t="n">
-        <v>-709.557402595866</v>
-      </c>
-    </row>
-    <row r="140">
+      <c r="G139">
+        <v>-709.55740259586605</v>
+      </c>
+    </row>
+    <row r="140" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F140" t="s">
         <v>38</v>
       </c>
-      <c r="G140" t="n">
+      <c r="G140">
         <v>-940.9917570050643</v>
       </c>
     </row>
-    <row r="141">
+    <row r="141" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F141" t="s">
         <v>25</v>
       </c>
-      <c r="G141" t="n">
-        <v>-1340.39064813006</v>
-      </c>
-    </row>
-    <row r="142">
+      <c r="G141">
+        <v>-1340.3906481300601</v>
+      </c>
+    </row>
+    <row r="142" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D142" t="s">
         <v>103</v>
       </c>
-      <c r="G142" t="n">
+      <c r="G142">
         <v>-10864.455537592065</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E143" t="s">
         <v>104</v>
       </c>
-      <c r="G143" t="n">
-        <v>-319.2613085236661</v>
-      </c>
-      <c r="H143" t="n">
-        <v>-308.4242518656725</v>
-      </c>
-    </row>
-    <row r="144">
+      <c r="G143">
+        <v>-319.26130852366612</v>
+      </c>
+      <c r="H143">
+        <v>-308.42425186567249</v>
+      </c>
+    </row>
+    <row r="144" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E144" t="s">
         <v>105</v>
       </c>
-      <c r="G144" t="n">
-        <v>-423.9192149384097</v>
-      </c>
-      <c r="H144" t="n">
-        <v>-356.324684509558</v>
-      </c>
-    </row>
-    <row r="145">
+      <c r="G144">
+        <v>-423.91921493840971</v>
+      </c>
+      <c r="H144">
+        <v>-356.32468450955798</v>
+      </c>
+    </row>
+    <row r="145" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E145" t="s">
         <v>106</v>
       </c>
-      <c r="G145" t="n">
-        <v>-628.8419299643282</v>
-      </c>
-      <c r="H145" t="n">
+      <c r="G145">
+        <v>-628.84192996432819</v>
+      </c>
+      <c r="H145">
         <v>-543.5740314890769</v>
       </c>
     </row>
-    <row r="146">
+    <row r="146" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E146" t="s">
         <v>107</v>
       </c>
-      <c r="G146" t="n">
-        <v>-724.3327467374854</v>
-      </c>
-      <c r="H146" t="n">
-        <v>-622.7420172279149</v>
-      </c>
-    </row>
-    <row r="147">
+      <c r="G146">
+        <v>-724.33274673748542</v>
+      </c>
+      <c r="H146">
+        <v>-622.74201722791486</v>
+      </c>
+    </row>
+    <row r="147" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E147" t="s">
         <v>108</v>
       </c>
-      <c r="G147" t="n">
+      <c r="G147">
         <v>-6854.3172788011025</v>
       </c>
-      <c r="H147" t="n">
-        <v>-5985.798603422271</v>
-      </c>
-    </row>
-    <row r="148">
+      <c r="H147">
+        <v>-5985.7986034222713</v>
+      </c>
+    </row>
+    <row r="148" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F148" t="s">
         <v>61</v>
       </c>
-      <c r="G148" t="n">
-        <v>-726.8617886009117</v>
-      </c>
-    </row>
-    <row r="149">
+      <c r="G148">
+        <v>-726.86178860091172</v>
+      </c>
+    </row>
+    <row r="149" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D149" t="s">
         <v>64</v>
       </c>
-      <c r="G149" t="n">
-        <v>-58795.74045882648</v>
-      </c>
-      <c r="H149" t="n">
-        <v>-81.47846239532909</v>
-      </c>
-    </row>
-    <row r="150">
+      <c r="G149">
+        <v>-58795.740458826484</v>
+      </c>
+      <c r="H149">
+        <v>-81.478462395329089</v>
+      </c>
+    </row>
+    <row r="150" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E150" t="s">
         <v>109</v>
       </c>
-      <c r="G150" t="n">
-        <v>-355.028375048966</v>
-      </c>
-      <c r="H150" t="n">
+      <c r="G150">
+        <v>-355.02837504896598</v>
+      </c>
+      <c r="H150">
         <v>-284.64530278531254</v>
       </c>
     </row>
-    <row r="151">
+    <row r="151" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E151" t="s">
         <v>110</v>
       </c>
-      <c r="G151" t="n">
-        <v>-528.907344117751</v>
-      </c>
-      <c r="H151" t="n">
+      <c r="G151">
+        <v>-528.90734411775099</v>
+      </c>
+      <c r="H151">
         <v>-458.54154723098475</v>
       </c>
     </row>
-    <row r="152">
+    <row r="152" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E152" t="s">
         <v>111</v>
       </c>
-      <c r="G152" t="n">
-        <v>-652.0173928173679</v>
-      </c>
-      <c r="H152" t="n">
+      <c r="G152">
+        <v>-652.01739281736786</v>
+      </c>
+      <c r="H152">
         <v>-325.3178885282328</v>
       </c>
     </row>
-    <row r="153">
+    <row r="153" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F153" t="s">
         <v>112</v>
       </c>
-      <c r="G153" t="n">
-        <v>-326.4383421464786</v>
-      </c>
-    </row>
-    <row r="154">
+      <c r="G153">
+        <v>-326.43834214647859</v>
+      </c>
+    </row>
+    <row r="154" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E154" t="s">
         <v>113</v>
       </c>
-      <c r="G154" t="n">
-        <v>-757.3352394820436</v>
-      </c>
-      <c r="H154" t="n">
-        <v>-608.7480493063063</v>
-      </c>
-    </row>
-    <row r="155">
+      <c r="G154">
+        <v>-757.33523948204356</v>
+      </c>
+      <c r="H154">
+        <v>-608.74804930630626</v>
+      </c>
+    </row>
+    <row r="155" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E155" t="s">
         <v>114</v>
       </c>
-      <c r="G155" t="n">
+      <c r="G155">
         <v>-1511.2609961933376</v>
       </c>
     </row>
-    <row r="156">
+    <row r="156" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F156" t="s">
         <v>80</v>
       </c>
-      <c r="G156" t="n">
+      <c r="G156">
         <v>-1511.2609961933376</v>
       </c>
-      <c r="H156" t="n">
-        <v>-3.157244522215288</v>
-      </c>
-    </row>
-    <row r="157">
+      <c r="H156">
+        <v>-3.1572445222152878</v>
+      </c>
+    </row>
+    <row r="157" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E157" t="s">
         <v>65</v>
       </c>
-      <c r="G157" t="n">
-        <v>-2359.993131765589</v>
-      </c>
-      <c r="H157" t="n">
-        <v>-2359.515122463169</v>
-      </c>
-    </row>
-    <row r="158">
+      <c r="G157">
+        <v>-2359.9931317655892</v>
+      </c>
+      <c r="H157">
+        <v>-2359.5151224631691</v>
+      </c>
+    </row>
+    <row r="158" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E158" t="s">
         <v>66</v>
       </c>
-      <c r="G158" t="n">
+      <c r="G158">
         <v>-21850.8725559628</v>
       </c>
-      <c r="H158" t="n">
-        <v>-21217.7744918958</v>
-      </c>
-    </row>
-    <row r="159">
+      <c r="H158">
+        <v>-21217.774491895801</v>
+      </c>
+    </row>
+    <row r="159" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F159" t="s">
         <v>115</v>
       </c>
-      <c r="G159" t="n">
+      <c r="G159">
         <v>-492.17780376936327</v>
       </c>
     </row>
-    <row r="160">
+    <row r="160" spans="4:8" x14ac:dyDescent="0.3">
       <c r="E160" t="s">
         <v>67</v>
       </c>
-      <c r="G160" t="n">
+      <c r="G160">
         <v>-29834.054337871734</v>
       </c>
-      <c r="H160" t="n">
-        <v>-25649.70210740299</v>
-      </c>
-    </row>
-    <row r="161">
+      <c r="H160">
+        <v>-25649.702107402991</v>
+      </c>
+    </row>
+    <row r="161" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F161" t="s">
         <v>61</v>
       </c>
-      <c r="G161" t="n">
-        <v>-4029.049081791805</v>
+      <c r="G161">
+        <v>-4029.0490817918048</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>